<commit_message>
completed with datatype check for both inputs & response
</commit_message>
<xml_diff>
--- a/input_data/payload/create_employee/create_emp.xlsx
+++ b/input_data/payload/create_employee/create_emp.xlsx
@@ -34,31 +34,31 @@
     <t xml:space="preserve">create_emloyee_with_empty_data</t>
   </si>
   <si>
-    <t xml:space="preserve">create_emloyee_with_valid_data.json</t>
-  </si>
-  <si>
-    <t xml:space="preserve">positive</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> create_emloyee_with_existing_name</t>
+    <t xml:space="preserve">create_emloyee_with_empty_data.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_emloyee_with_existing_name</t>
   </si>
   <si>
     <t xml:space="preserve">create_emloyee_with_existing_name.json</t>
   </si>
   <si>
-    <t xml:space="preserve">negative</t>
-  </si>
-  <si>
     <t xml:space="preserve">create_emloyee_with_invalid_data_types</t>
   </si>
   <si>
     <t xml:space="preserve">create_emloyee_with_invalid_data_types.json</t>
   </si>
   <si>
-    <t xml:space="preserve">create_emloyee_with_valid_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create_emloyee_with_empty_data.json</t>
+    <t>create_emloyee_with_valid_data</t>
+  </si>
+  <si>
+    <t>create_emloyee_with_valid_data.json</t>
+  </si>
+  <si>
+    <t>positive</t>
   </si>
 </sst>
 </file>
@@ -159,21 +159,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="5:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col min="1" max="1" hidden="false" style="0" width="36.1785714285714" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="36.719387755102" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="11.8775510204082" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="18.0867346938776" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="8.23469387755102" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="38.8775510204082" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="8.23469387755102" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -207,29 +207,29 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>